<commit_message>
updating the flood delay experiment files. adding fastq file names as well as ensuring consistent keys and paths
</commit_message>
<xml_diff>
--- a/bioSample/bioSample_J.PLAGGENBERG_06.06.19.xlsx
+++ b/bioSample/bioSample_J.PLAGGENBERG_06.06.19.xlsx
@@ -1,12 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessicaplaggenberg/Documents/rnaseq-database/bioSample/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4111F06D-68E4-1E45-B12D-8A425F38949E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="560" windowWidth="21700" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -76,82 +95,388 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:Z37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -203,7 +528,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -211,7 +536,7 @@
         <v>13</v>
       </c>
       <c r="C2" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>14</v>
@@ -223,19 +548,19 @@
         <v>16</v>
       </c>
       <c r="I2" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K2" s="5">
-        <v>-1.0</v>
+        <v>-1</v>
       </c>
       <c r="L2" s="6">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>12</v>
       </c>
@@ -243,7 +568,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="3">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>14</v>
@@ -255,19 +580,19 @@
         <v>16</v>
       </c>
       <c r="I3" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K3" s="5">
-        <v>-1.0</v>
+        <v>-1</v>
       </c>
       <c r="L3" s="6">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
@@ -275,7 +600,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="3">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>14</v>
@@ -287,19 +612,19 @@
         <v>16</v>
       </c>
       <c r="I4" s="5">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K4" s="5">
-        <v>-1.0</v>
+        <v>-1</v>
       </c>
       <c r="L4" s="6">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>12</v>
       </c>
@@ -307,7 +632,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>14</v>
@@ -319,19 +644,19 @@
         <v>19</v>
       </c>
       <c r="I5" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K5" s="5">
-        <v>-1.0</v>
+        <v>-1</v>
       </c>
       <c r="L5" s="6">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
@@ -339,7 +664,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>14</v>
@@ -351,19 +676,19 @@
         <v>19</v>
       </c>
       <c r="I6" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K6" s="5">
-        <v>-1.0</v>
+        <v>-1</v>
       </c>
       <c r="L6" s="6">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
@@ -371,7 +696,7 @@
         <v>13</v>
       </c>
       <c r="C7" s="3">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>14</v>
@@ -383,19 +708,19 @@
         <v>19</v>
       </c>
       <c r="I7" s="5">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K7" s="5">
-        <v>-1.0</v>
+        <v>-1</v>
       </c>
       <c r="L7" s="6">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
@@ -403,7 +728,7 @@
         <v>13</v>
       </c>
       <c r="C8" s="3">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>14</v>
@@ -415,19 +740,19 @@
         <v>16</v>
       </c>
       <c r="I8" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K8" s="5">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="L8" s="6">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
@@ -435,7 +760,7 @@
         <v>13</v>
       </c>
       <c r="C9" s="3">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>14</v>
@@ -447,19 +772,19 @@
         <v>16</v>
       </c>
       <c r="I9" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K9" s="5">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="L9" s="6">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
@@ -467,7 +792,7 @@
         <v>13</v>
       </c>
       <c r="C10" s="3">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>14</v>
@@ -479,19 +804,19 @@
         <v>16</v>
       </c>
       <c r="I10" s="5">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K10" s="5">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="L10" s="6">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
@@ -499,7 +824,7 @@
         <v>13</v>
       </c>
       <c r="C11" s="3">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>14</v>
@@ -511,19 +836,19 @@
         <v>19</v>
       </c>
       <c r="I11" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K11" s="5">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="L11" s="6">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>12</v>
       </c>
@@ -531,7 +856,7 @@
         <v>13</v>
       </c>
       <c r="C12" s="3">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>14</v>
@@ -543,19 +868,19 @@
         <v>19</v>
       </c>
       <c r="I12" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K12" s="5">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="L12" s="6">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
@@ -563,7 +888,7 @@
         <v>13</v>
       </c>
       <c r="C13" s="3">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>14</v>
@@ -575,91 +900,91 @@
         <v>19</v>
       </c>
       <c r="I13" s="5">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K13" s="5">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="L13" s="6">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
     </row>
-    <row r="29">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
     </row>
-    <row r="30">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
     </row>
-    <row r="31">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" s="4"/>
     </row>
-    <row r="32">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" s="4"/>
     </row>
-    <row r="33">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="4"/>
     </row>
-    <row r="34">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="4"/>
     </row>
-    <row r="35">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="4"/>
     </row>
-    <row r="36">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="4"/>
     </row>
-    <row r="37">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" s="4"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>